<commit_message>
updated COPYcorechoices_MSPF.xlsx with dates to exclude from MD98-2181 as described by Stott (2007)
</commit_message>
<xml_diff>
--- a/COPYcorechoices_MSPF.xlsx
+++ b/COPYcorechoices_MSPF.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samnewall/Documents/MATLAB/CoreSpreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samnewall/Documents/MATLAB/nSRdist_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B080643-FB13-CE4E-B099-3F4E97F399CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B28ED28E-DCC9-BD4A-BC65-5A75B3FBE7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6620" yWindow="500" windowWidth="43180" windowHeight="20440" xr2:uid="{4BD1B51B-9356-FE41-9D04-E60CF7F4E590}"/>
+    <workbookView xWindow="51200" yWindow="2420" windowWidth="28800" windowHeight="27020" xr2:uid="{4BD1B51B-9356-FE41-9D04-E60CF7F4E590}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1796" uniqueCount="851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1797" uniqueCount="852">
   <si>
     <t xml:space="preserve">Core Name </t>
   </si>
@@ -2592,6 +2592,9 @@
   </si>
   <si>
     <t>2329, SUERC-25165, SUERC-25166, SUERC-25167, 2331, SUERC-25170, SUERC-25171, SUERC-25172, 2332, 3818, 2333, 12329, 2335, 3823, 12335, 12337, 2336, 2337, 2414, 2416, 2417, 2418, 3825, SUERC-25631</t>
+  </si>
+  <si>
+    <t>OS-49938, OS-51038, OS-51309, OS-38541, OS-40505, OS-47068, OS-35980, OS-38542, OS-49298, OS-34877</t>
   </si>
 </sst>
 </file>
@@ -2946,10 +2949,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC11D6D-924D-B041-B64E-4010271A21B7}">
   <dimension ref="A1:V299"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="118" workbookViewId="0">
       <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection activeCell="A36" sqref="A36"/>
-      <selection pane="topRight" activeCell="K176" sqref="K176"/>
+      <selection pane="topRight" activeCell="Y199" sqref="Y199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10324,6 +10327,9 @@
       <c r="O195" t="s">
         <v>620</v>
       </c>
+      <c r="S195" t="s">
+        <v>851</v>
+      </c>
     </row>
     <row r="196" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A196" t="s">

</xml_diff>

<commit_message>
fixed a problem for core MD99-2343 (incDepth information was actually in LabID location, leading to problem reading in data to code).
</commit_message>
<xml_diff>
--- a/COPYcorechoices_MSPF.xlsx
+++ b/COPYcorechoices_MSPF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samnewall/Documents/MATLAB/nSRdist_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B28ED28E-DCC9-BD4A-BC65-5A75B3FBE7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CB3B69E-32F3-4345-99F3-0D2F76ABB0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="2420" windowWidth="28800" windowHeight="27020" xr2:uid="{4BD1B51B-9356-FE41-9D04-E60CF7F4E590}"/>
   </bookViews>
@@ -2949,10 +2949,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC11D6D-924D-B041-B64E-4010271A21B7}">
   <dimension ref="A1:V299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="118" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="118" workbookViewId="0">
       <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection activeCell="A36" sqref="A36"/>
-      <selection pane="topRight" activeCell="Y199" sqref="Y199"/>
+      <selection pane="topRight" activeCell="P197" sqref="P197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10406,7 +10406,7 @@
       <c r="N197" t="s">
         <v>614</v>
       </c>
-      <c r="O197" t="s">
+      <c r="P197" t="s">
         <v>685</v>
       </c>
       <c r="U197" t="s">

</xml_diff>

<commit_message>
updated a few comments
</commit_message>
<xml_diff>
--- a/COPYcorechoices_MSPF.xlsx
+++ b/COPYcorechoices_MSPF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samnewall/Documents/MATLAB/nSRdist_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CB3B69E-32F3-4345-99F3-0D2F76ABB0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F53265F0-3554-064D-AE0D-FCDF1FAD5C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="2420" windowWidth="28800" windowHeight="27020" xr2:uid="{4BD1B51B-9356-FE41-9D04-E60CF7F4E590}"/>
+    <workbookView xWindow="51860" yWindow="2340" windowWidth="27740" windowHeight="26960" xr2:uid="{4BD1B51B-9356-FE41-9D04-E60CF7F4E590}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1797" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1796" uniqueCount="851">
   <si>
     <t xml:space="preserve">Core Name </t>
   </si>
@@ -2036,9 +2036,6 @@
     <t>Planktonic Foraminifera, but last age is actually a tephra age</t>
   </si>
   <si>
-    <t>Radiocarbon age with CAMS100676 has been reported twice for this core (once with depth 3.0775 and once with depth 3.08 - the latter is unlabeled in PDV) Most of the missing Lab IDs are available in Williams et al., 2010</t>
-  </si>
-  <si>
     <t>CAMS100676</t>
   </si>
   <si>
@@ -2531,9 +2528,6 @@
     <t>Use Comments</t>
   </si>
   <si>
-    <t>Not sure why not used…</t>
-  </si>
-  <si>
     <t>﻿Dang, H., Jian, Z., Kissel, C., and Bassinot, F.: Precessional changes in the western equatorial Pacific Hydroclimate: A 240 kyr marine record from the Halmahera Sea, East Indonesia, Geochem. Geophys. Geosyst., 16, 148-164, doi:10.1002/2014GC005550, 2015.</t>
   </si>
   <si>
@@ -2595,6 +2589,9 @@
   </si>
   <si>
     <t>OS-49938, OS-51038, OS-51309, OS-38541, OS-40505, OS-47068, OS-35980, OS-38542, OS-49298, OS-34877</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radiocarbon age with CAMS100676 has been reported twice for this core (once with depth 3.0775 and once with depth 3.08 - the latter is unlabeled in PDV) Most of the missing Lab IDs are available in Williams et al., 2010. I remove the shallower of these repeated dates because it comes from LoDico et al., 2006, and unfortunately has a 400y offset already applied within WA2022. The shallower 6 dates also have this 400y offset, but I keep them as it doesn't seem to affect too much. I mentioned this double-reporting problem to Mulitza and he noticed the age offset problem and has corrected it for his new Atlas. </t>
   </si>
 </sst>
 </file>
@@ -2949,10 +2946,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC11D6D-924D-B041-B64E-4010271A21B7}">
   <dimension ref="A1:V299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="118" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
       <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection activeCell="A36" sqref="A36"/>
-      <selection pane="topRight" activeCell="P197" sqref="P197"/>
+      <selection pane="topRight" activeCell="K176" sqref="K176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2970,7 +2967,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -2985,16 +2982,16 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="K1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="L1" t="s">
         <v>641</v>
@@ -3027,7 +3024,7 @@
         <v>644</v>
       </c>
       <c r="V1" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -3035,7 +3032,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D2">
         <v>-75.932998657226506</v>
@@ -3068,10 +3065,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C3" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D3">
         <v>126.980003356933</v>
@@ -3109,10 +3106,10 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C4" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D4">
         <v>72.652000427246094</v>
@@ -3150,7 +3147,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D5">
         <v>-119.8570022583</v>
@@ -3183,7 +3180,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D6">
         <v>-118.41699981689401</v>
@@ -3216,7 +3213,7 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D7">
         <v>-118.11699676513599</v>
@@ -3249,7 +3246,7 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D8">
         <v>-119.059997558593</v>
@@ -3282,10 +3279,10 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C9" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D9">
         <v>14.029999732971101</v>
@@ -3318,7 +3315,7 @@
         <v>640</v>
       </c>
       <c r="U9" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
@@ -3326,7 +3323,7 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D10">
         <v>5.5669999122619602</v>
@@ -3359,7 +3356,7 @@
         <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D11">
         <v>179.99699401855401</v>
@@ -3392,7 +3389,7 @@
         <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D12">
         <v>-171.5</v>
@@ -3425,7 +3422,7 @@
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D13">
         <v>-91.349998474121094</v>
@@ -3463,10 +3460,10 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C14" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D14">
         <v>-44.194999694824197</v>
@@ -3504,10 +3501,10 @@
         <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C15" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D15">
         <v>-44.470001220703097</v>
@@ -3545,10 +3542,10 @@
         <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C16" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D16">
         <v>-44.259998321533203</v>
@@ -3584,7 +3581,7 @@
         <v>631</v>
       </c>
       <c r="U16" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
@@ -3592,7 +3589,7 @@
         <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D17">
         <v>-117.583000183105</v>
@@ -3625,7 +3622,7 @@
         <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D18">
         <v>-117.36699676513599</v>
@@ -3658,7 +3655,7 @@
         <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D19">
         <v>-118.400001525878</v>
@@ -3691,7 +3688,7 @@
         <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D20">
         <v>-118.133003234863</v>
@@ -3724,7 +3721,7 @@
         <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D21">
         <v>-118.800003051757</v>
@@ -3757,7 +3754,7 @@
         <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D22">
         <v>-119.949996948242</v>
@@ -3790,7 +3787,7 @@
         <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D23">
         <v>-123.24299621582</v>
@@ -3823,7 +3820,7 @@
         <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D24">
         <v>4.4499998092651296</v>
@@ -3856,7 +3853,7 @@
         <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D25">
         <v>162.55799865722599</v>
@@ -3891,7 +3888,7 @@
         <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D26">
         <v>146.891998291015</v>
@@ -3924,7 +3921,7 @@
         <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D27">
         <v>147.42999267578099</v>
@@ -3957,7 +3954,7 @@
         <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D28">
         <v>145.94999694824199</v>
@@ -3990,10 +3987,10 @@
         <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C29" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D29">
         <v>147.74200439453099</v>
@@ -4031,7 +4028,7 @@
         <v>67</v>
       </c>
       <c r="B30" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D30">
         <v>103.246002197265</v>
@@ -4064,7 +4061,7 @@
         <v>69</v>
       </c>
       <c r="B31" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D31">
         <v>112.87200164794901</v>
@@ -4097,7 +4094,7 @@
         <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D32">
         <v>120.91699981689401</v>
@@ -4130,7 +4127,7 @@
         <v>73</v>
       </c>
       <c r="B33" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D33">
         <v>10.9519996643066</v>
@@ -4163,10 +4160,10 @@
         <v>75</v>
       </c>
       <c r="B34" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C34" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D34">
         <v>11.012000083923301</v>
@@ -4196,10 +4193,10 @@
         <v>614</v>
       </c>
       <c r="O34" t="s">
+        <v>714</v>
+      </c>
+      <c r="U34" t="s">
         <v>715</v>
-      </c>
-      <c r="U34" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.2">
@@ -4207,7 +4204,7 @@
         <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D35">
         <v>-12.428000450134199</v>
@@ -4240,7 +4237,7 @@
         <v>79</v>
       </c>
       <c r="B36" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D36">
         <v>-12.428000450134199</v>
@@ -4273,7 +4270,7 @@
         <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D37">
         <v>-29.656999588012599</v>
@@ -4306,7 +4303,7 @@
         <v>83</v>
       </c>
       <c r="B38" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D38">
         <v>-18.004999160766602</v>
@@ -4339,10 +4336,10 @@
         <v>85</v>
       </c>
       <c r="B39" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C39" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D39">
         <v>-53.744998931884702</v>
@@ -4380,10 +4377,10 @@
         <v>87</v>
       </c>
       <c r="B40" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C40" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D40">
         <v>-30.646999359130799</v>
@@ -4421,10 +4418,10 @@
         <v>89</v>
       </c>
       <c r="B41" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C41" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D41">
         <v>-43.666999816894503</v>
@@ -4462,7 +4459,7 @@
         <v>91</v>
       </c>
       <c r="B42" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D42">
         <v>-41.591999053955</v>
@@ -4498,10 +4495,10 @@
         <v>93</v>
       </c>
       <c r="B43" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C43" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D43">
         <v>-43.023998260497997</v>
@@ -4539,7 +4536,7 @@
         <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D44">
         <v>-52.083000183105398</v>
@@ -4575,10 +4572,10 @@
         <v>97</v>
       </c>
       <c r="B45" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C45" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D45">
         <v>12.3769998550415</v>
@@ -4614,10 +4611,10 @@
         <v>1.375</v>
       </c>
       <c r="S45" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="U45" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.2">
@@ -4625,10 +4622,10 @@
         <v>99</v>
       </c>
       <c r="B46" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C46" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D46">
         <v>13.8350000381469</v>
@@ -4666,10 +4663,10 @@
         <v>101</v>
       </c>
       <c r="B47" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C47" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="D47">
         <v>-46.373001098632798</v>
@@ -4707,10 +4704,10 @@
         <v>103</v>
       </c>
       <c r="B48" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C48" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D48">
         <v>-46.451999664306598</v>
@@ -4748,10 +4745,10 @@
         <v>105</v>
       </c>
       <c r="B49" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C49" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D49">
         <v>-45.881999969482401</v>
@@ -4787,7 +4784,7 @@
         <v>632</v>
       </c>
       <c r="U49" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.2">
@@ -4795,7 +4792,7 @@
         <v>107</v>
       </c>
       <c r="B50" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D50">
         <v>-34.022998809814403</v>
@@ -4828,7 +4825,7 @@
         <v>109</v>
       </c>
       <c r="B51" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D51">
         <v>-34.021999359130803</v>
@@ -4856,7 +4853,7 @@
       </c>
       <c r="T51"/>
       <c r="U51" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.2">
@@ -4864,10 +4861,10 @@
         <v>111</v>
       </c>
       <c r="B52" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C52" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="D52">
         <v>-39.978000640869098</v>
@@ -4905,7 +4902,7 @@
         <v>113</v>
       </c>
       <c r="B53" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D53">
         <v>-72.089996337890597</v>
@@ -4941,10 +4938,10 @@
         <v>115</v>
       </c>
       <c r="B54" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C54" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="D54">
         <v>-72.192001342773395</v>
@@ -4982,10 +4979,10 @@
         <v>117</v>
       </c>
       <c r="B55" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C55" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="D55">
         <v>-72.016998291015597</v>
@@ -5023,7 +5020,7 @@
         <v>119</v>
       </c>
       <c r="B56" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D56">
         <v>-71.251998901367102</v>
@@ -5056,7 +5053,7 @@
         <v>121</v>
       </c>
       <c r="B57" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D57">
         <v>13.083000183105399</v>
@@ -5086,10 +5083,10 @@
         <v>619</v>
       </c>
       <c r="O57" t="s">
+        <v>710</v>
+      </c>
+      <c r="U57" t="s">
         <v>711</v>
-      </c>
-      <c r="U57" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.2">
@@ -5097,7 +5094,7 @@
         <v>123</v>
       </c>
       <c r="B58" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D58">
         <v>12.022000312805099</v>
@@ -5125,7 +5122,7 @@
       </c>
       <c r="T58"/>
       <c r="U58" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.2">
@@ -5133,10 +5130,10 @@
         <v>125</v>
       </c>
       <c r="B59" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C59" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D59">
         <v>-58.330001831054602</v>
@@ -5174,7 +5171,7 @@
         <v>127</v>
       </c>
       <c r="B60" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D60">
         <v>-13.2250003814697</v>
@@ -5204,10 +5201,10 @@
         <v>619</v>
       </c>
       <c r="O60" t="s">
+        <v>712</v>
+      </c>
+      <c r="U60" t="s">
         <v>713</v>
-      </c>
-      <c r="U60" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.2">
@@ -5215,7 +5212,7 @@
         <v>129</v>
       </c>
       <c r="B61" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D61">
         <v>-15.4519996643066</v>
@@ -5253,10 +5250,10 @@
         <v>131</v>
       </c>
       <c r="B62" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C62" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D62">
         <v>9.3900003433227504</v>
@@ -5286,7 +5283,7 @@
         <v>612</v>
       </c>
       <c r="O62" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.2">
@@ -5294,10 +5291,10 @@
         <v>133</v>
       </c>
       <c r="B63" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C63" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="D63">
         <v>-53.965000152587798</v>
@@ -5335,10 +5332,10 @@
         <v>135</v>
       </c>
       <c r="B64" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C64" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D64">
         <v>-53.205001831054602</v>
@@ -5376,7 +5373,7 @@
         <v>137</v>
       </c>
       <c r="B65" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D65">
         <v>-70.823997497558594</v>
@@ -5409,7 +5406,7 @@
         <v>139</v>
       </c>
       <c r="B66" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D66">
         <v>-18.5820007324218</v>
@@ -5437,7 +5434,7 @@
       </c>
       <c r="T66"/>
       <c r="U66" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
@@ -5445,10 +5442,10 @@
         <v>141</v>
       </c>
       <c r="B67" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C67" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D67">
         <v>-18.451999664306602</v>
@@ -5486,10 +5483,10 @@
         <v>143</v>
       </c>
       <c r="B68" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C68" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D68">
         <v>-18.099000930786101</v>
@@ -5527,7 +5524,7 @@
         <v>145</v>
       </c>
       <c r="B69" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D69">
         <v>-18.350000381469702</v>
@@ -5560,7 +5557,7 @@
         <v>147</v>
       </c>
       <c r="B70" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D70">
         <v>-17.947999954223601</v>
@@ -5596,7 +5593,7 @@
         <v>149</v>
       </c>
       <c r="B71" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D71">
         <v>-17.652999877929599</v>
@@ -5629,7 +5626,7 @@
         <v>151</v>
       </c>
       <c r="B72" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D72">
         <v>-18.056999206542901</v>
@@ -5662,7 +5659,7 @@
         <v>153</v>
       </c>
       <c r="B73" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D73">
         <v>-20.659000396728501</v>
@@ -5695,7 +5692,7 @@
         <v>155</v>
       </c>
       <c r="B74" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D74">
         <v>-31.841999053955</v>
@@ -5736,7 +5733,7 @@
         <v>157</v>
       </c>
       <c r="B75" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D75">
         <v>139.5</v>
@@ -5774,10 +5771,10 @@
         <v>159</v>
       </c>
       <c r="B76" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C76" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D76">
         <v>-18.0090007781982</v>
@@ -5815,7 +5812,7 @@
         <v>161</v>
       </c>
       <c r="B77" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D77">
         <v>-18.9869995117187</v>
@@ -5851,7 +5848,7 @@
         <v>163</v>
       </c>
       <c r="B78" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D78">
         <v>-7.8150000572204501</v>
@@ -5884,7 +5881,7 @@
         <v>165</v>
       </c>
       <c r="B79" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D79">
         <v>-7.5760002136230398</v>
@@ -5917,7 +5914,7 @@
         <v>167</v>
       </c>
       <c r="B80" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D80">
         <v>-10.647000312805099</v>
@@ -5950,10 +5947,10 @@
         <v>169</v>
       </c>
       <c r="B81" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C81" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D81">
         <v>37.869998931884702</v>
@@ -5983,10 +5980,10 @@
         <v>612</v>
       </c>
       <c r="O81" t="s">
+        <v>695</v>
+      </c>
+      <c r="U81" t="s">
         <v>696</v>
-      </c>
-      <c r="U81" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.2">
@@ -5994,7 +5991,7 @@
         <v>171</v>
       </c>
       <c r="B82" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D82">
         <v>89.878997802734304</v>
@@ -6030,7 +6027,7 @@
         <v>174</v>
       </c>
       <c r="B83" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D83">
         <v>-72.032997131347599</v>
@@ -6063,7 +6060,7 @@
         <v>176</v>
       </c>
       <c r="B84" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D84">
         <v>117.383003234863</v>
@@ -6093,7 +6090,7 @@
         <v>608</v>
       </c>
       <c r="U84" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.2">
@@ -6101,10 +6098,10 @@
         <v>178</v>
       </c>
       <c r="B85" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C85" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D85">
         <v>112.33200073242099</v>
@@ -6142,10 +6139,10 @@
         <v>180</v>
       </c>
       <c r="B86" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C86" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D86">
         <v>112.212997436523</v>
@@ -6183,7 +6180,7 @@
         <v>182</v>
       </c>
       <c r="B87" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D87">
         <v>118.113998413085</v>
@@ -6213,10 +6210,10 @@
         <v>612</v>
       </c>
       <c r="O87" t="s">
+        <v>673</v>
+      </c>
+      <c r="U87" t="s">
         <v>674</v>
-      </c>
-      <c r="U87" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.2">
@@ -6224,10 +6221,10 @@
         <v>184</v>
       </c>
       <c r="B88" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C88" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D88">
         <v>118.16699981689401</v>
@@ -6257,10 +6254,10 @@
         <v>612</v>
       </c>
       <c r="O88" t="s">
+        <v>716</v>
+      </c>
+      <c r="U88" t="s">
         <v>717</v>
-      </c>
-      <c r="U88" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.2">
@@ -6268,10 +6265,10 @@
         <v>186</v>
       </c>
       <c r="B89" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C89" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D89">
         <v>119.583000183105</v>
@@ -6301,10 +6298,10 @@
         <v>612</v>
       </c>
       <c r="O89" t="s">
+        <v>718</v>
+      </c>
+      <c r="U89" t="s">
         <v>719</v>
-      </c>
-      <c r="U89" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.2">
@@ -6312,10 +6309,10 @@
         <v>188</v>
       </c>
       <c r="B90" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C90" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D90">
         <v>-42.509998321533203</v>
@@ -6353,7 +6350,7 @@
         <v>190</v>
       </c>
       <c r="B91" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D91">
         <v>-43.402000427246001</v>
@@ -6386,7 +6383,7 @@
         <v>192</v>
       </c>
       <c r="B92" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D92">
         <v>-40.042999267578097</v>
@@ -6419,7 +6416,7 @@
         <v>194</v>
       </c>
       <c r="B93" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D93">
         <v>-40.022998809814403</v>
@@ -6452,7 +6449,7 @@
         <v>196</v>
       </c>
       <c r="B94" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D94">
         <v>-42.617000579833899</v>
@@ -6490,10 +6487,10 @@
         <v>198</v>
       </c>
       <c r="B95" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C95" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D95">
         <v>-37.075000762939403</v>
@@ -6531,7 +6528,7 @@
         <v>200</v>
       </c>
       <c r="B96" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D96">
         <v>177.44000244140599</v>
@@ -6569,10 +6566,10 @@
         <v>202</v>
       </c>
       <c r="B97" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C97" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D97">
         <v>-4.2729997634887598</v>
@@ -6602,10 +6599,10 @@
         <v>614</v>
       </c>
       <c r="P97" t="s">
+        <v>720</v>
+      </c>
+      <c r="U97" t="s">
         <v>721</v>
-      </c>
-      <c r="U97" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.2">
@@ -6613,10 +6610,10 @@
         <v>204</v>
       </c>
       <c r="B98" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C98" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D98">
         <v>112.7320022583</v>
@@ -6646,7 +6643,7 @@
         <v>608</v>
       </c>
       <c r="O98" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.2">
@@ -6654,7 +6651,7 @@
         <v>206</v>
       </c>
       <c r="B99" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D99">
         <v>18.530000686645501</v>
@@ -6687,7 +6684,7 @@
         <v>208</v>
       </c>
       <c r="B100" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D100">
         <v>-46.126998901367102</v>
@@ -6720,7 +6717,7 @@
         <v>210</v>
       </c>
       <c r="B101" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D101">
         <v>-26.444999694824201</v>
@@ -6753,7 +6750,7 @@
         <v>212</v>
       </c>
       <c r="B102" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D102">
         <v>-21.923000335693299</v>
@@ -6786,7 +6783,7 @@
         <v>214</v>
       </c>
       <c r="B103" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D103">
         <v>-15.958000183105399</v>
@@ -6819,7 +6816,7 @@
         <v>216</v>
       </c>
       <c r="B104" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D104">
         <v>-13.390000343322701</v>
@@ -6852,7 +6849,7 @@
         <v>218</v>
       </c>
       <c r="B105" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D105">
         <v>-13.8470001220703</v>
@@ -6885,7 +6882,7 @@
         <v>220</v>
       </c>
       <c r="B106" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D106">
         <v>-14.9600000381469</v>
@@ -6918,7 +6915,7 @@
         <v>222</v>
       </c>
       <c r="B107" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D107">
         <v>-16.211999893188398</v>
@@ -6951,10 +6948,10 @@
         <v>224</v>
       </c>
       <c r="B108" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C108" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D108">
         <v>12.765000343322701</v>
@@ -6992,7 +6989,7 @@
         <v>226</v>
       </c>
       <c r="B109" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D109">
         <v>12.3599996566772</v>
@@ -7022,7 +7019,7 @@
         <v>619</v>
       </c>
       <c r="O109" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.2">
@@ -7030,10 +7027,10 @@
         <v>228</v>
       </c>
       <c r="B110" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C110" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D110">
         <v>133.99499511718699</v>
@@ -7071,7 +7068,7 @@
         <v>231</v>
       </c>
       <c r="B111" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D111">
         <v>-39.279998779296797</v>
@@ -7109,7 +7106,7 @@
         <v>233</v>
       </c>
       <c r="B112" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D112">
         <v>143.36700439453099</v>
@@ -7142,7 +7139,7 @@
         <v>235</v>
       </c>
       <c r="B113" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D113">
         <v>-76.383003234863196</v>
@@ -7180,7 +7177,7 @@
         <v>237</v>
       </c>
       <c r="B114" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D114">
         <v>-76.289001464843693</v>
@@ -7218,7 +7215,7 @@
         <v>239</v>
       </c>
       <c r="B115" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D115">
         <v>-72.898002624511705</v>
@@ -7251,7 +7248,7 @@
         <v>241</v>
       </c>
       <c r="B116" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D116">
         <v>-74.410003662109304</v>
@@ -7289,7 +7286,7 @@
         <v>243</v>
       </c>
       <c r="B117" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D117">
         <v>-74.468002319335895</v>
@@ -7327,10 +7324,10 @@
         <v>245</v>
       </c>
       <c r="B118" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C118" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D118">
         <v>-75.416999816894503</v>
@@ -7360,7 +7357,7 @@
         <v>612</v>
       </c>
       <c r="O118" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="119" spans="1:21" x14ac:dyDescent="0.2">
@@ -7368,7 +7365,7 @@
         <v>247</v>
       </c>
       <c r="B119" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D119">
         <v>-76.067001342773395</v>
@@ -7406,7 +7403,7 @@
         <v>249</v>
       </c>
       <c r="B120" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D120">
         <v>-76.236000061035099</v>
@@ -7444,10 +7441,10 @@
         <v>251</v>
       </c>
       <c r="B121" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C121" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D121">
         <v>-76.286003112792898</v>
@@ -7485,7 +7482,7 @@
         <v>253</v>
       </c>
       <c r="B122" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D122">
         <v>-76.2969970703125</v>
@@ -7523,7 +7520,7 @@
         <v>255</v>
       </c>
       <c r="B123" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D123">
         <v>-76.126998901367102</v>
@@ -7561,7 +7558,7 @@
         <v>257</v>
       </c>
       <c r="B124" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D124">
         <v>-76.293998718261705</v>
@@ -7599,7 +7596,7 @@
         <v>259</v>
       </c>
       <c r="B125" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D125">
         <v>-76.128997802734304</v>
@@ -7637,10 +7634,10 @@
         <v>261</v>
       </c>
       <c r="B126" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C126" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D126">
         <v>-45.080001831054602</v>
@@ -7672,9 +7669,11 @@
       <c r="O126" t="s">
         <v>611</v>
       </c>
-      <c r="T126"/>
+      <c r="T126">
+        <v>0.995</v>
+      </c>
       <c r="U126" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="127" spans="1:21" x14ac:dyDescent="0.2">
@@ -7682,7 +7681,7 @@
         <v>263</v>
       </c>
       <c r="B127" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D127">
         <v>-46.483001708984297</v>
@@ -7718,7 +7717,7 @@
         <v>265</v>
       </c>
       <c r="B128" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D128">
         <v>-45.540000915527301</v>
@@ -7746,7 +7745,7 @@
       </c>
       <c r="T128"/>
       <c r="U128" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.2">
@@ -7754,7 +7753,7 @@
         <v>267</v>
       </c>
       <c r="B129" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D129">
         <v>-43.583000183105398</v>
@@ -7782,7 +7781,7 @@
       </c>
       <c r="T129"/>
       <c r="U129" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="130" spans="1:21" x14ac:dyDescent="0.2">
@@ -7790,7 +7789,7 @@
         <v>269</v>
       </c>
       <c r="B130" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D130">
         <v>-46.067001342773402</v>
@@ -7823,7 +7822,7 @@
         <v>271</v>
       </c>
       <c r="B131" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D131">
         <v>-46.180000305175703</v>
@@ -7856,7 +7855,7 @@
         <v>273</v>
       </c>
       <c r="B132" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D132">
         <v>-46.470001220703097</v>
@@ -7886,10 +7885,10 @@
         <v>612</v>
       </c>
       <c r="O132" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="U132" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.2">
@@ -7897,7 +7896,7 @@
         <v>275</v>
       </c>
       <c r="B133" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D133">
         <v>-46.630001068115199</v>
@@ -7930,7 +7929,7 @@
         <v>277</v>
       </c>
       <c r="B134" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D134">
         <v>-43.333000183105398</v>
@@ -7963,7 +7962,7 @@
         <v>279</v>
       </c>
       <c r="B135" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D135">
         <v>-45.840000152587798</v>
@@ -7996,7 +7995,7 @@
         <v>281</v>
       </c>
       <c r="B136" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D136">
         <v>-46.330001831054602</v>
@@ -8024,7 +8023,7 @@
       </c>
       <c r="T136"/>
       <c r="U136" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.2">
@@ -8032,7 +8031,7 @@
         <v>283</v>
       </c>
       <c r="B137" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D137">
         <v>-46.630001068115199</v>
@@ -8060,7 +8059,7 @@
       </c>
       <c r="T137"/>
       <c r="U137" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.2">
@@ -8068,10 +8067,10 @@
         <v>285</v>
       </c>
       <c r="B138" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C138" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D138">
         <v>-48.540000915527301</v>
@@ -8109,10 +8108,10 @@
         <v>287</v>
       </c>
       <c r="B139" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C139" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D139">
         <v>-52.790000915527301</v>
@@ -8142,10 +8141,10 @@
         <v>612</v>
       </c>
       <c r="O139" t="s">
+        <v>722</v>
+      </c>
+      <c r="U139" t="s">
         <v>723</v>
-      </c>
-      <c r="U139" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.2">
@@ -8153,7 +8152,7 @@
         <v>289</v>
       </c>
       <c r="B140" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D140">
         <v>-53.169998168945298</v>
@@ -8191,7 +8190,7 @@
         <v>291</v>
       </c>
       <c r="B141" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D141">
         <v>-53.2299995422363</v>
@@ -8229,7 +8228,7 @@
         <v>293</v>
       </c>
       <c r="B142" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D142">
         <v>-52.970001220703097</v>
@@ -8264,7 +8263,7 @@
         <v>295</v>
       </c>
       <c r="B143" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D143">
         <v>-53.680000305175703</v>
@@ -8299,10 +8298,10 @@
         <v>297</v>
       </c>
       <c r="B144" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C144" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D144">
         <v>-44.799999237060497</v>
@@ -8340,10 +8339,10 @@
         <v>299</v>
       </c>
       <c r="B145" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C145" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D145">
         <v>-43.2299995422363</v>
@@ -8381,7 +8380,7 @@
         <v>301</v>
       </c>
       <c r="B146" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D146">
         <v>-57.615001678466797</v>
@@ -8414,7 +8413,7 @@
         <v>617</v>
       </c>
       <c r="U146" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="147" spans="1:21" x14ac:dyDescent="0.2">
@@ -8422,10 +8421,10 @@
         <v>303</v>
       </c>
       <c r="B147" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C147" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D147">
         <v>-110.26799774169901</v>
@@ -8463,7 +8462,7 @@
         <v>305</v>
       </c>
       <c r="B148" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D148">
         <v>-114.18699645996</v>
@@ -8495,7 +8494,7 @@
         <v>307</v>
       </c>
       <c r="B149" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D149">
         <v>-2.1199998855590798</v>
@@ -8528,7 +8527,7 @@
         <v>309</v>
       </c>
       <c r="B150" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D150">
         <v>144.31700134277301</v>
@@ -8566,7 +8565,7 @@
         <v>311</v>
       </c>
       <c r="B151" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D151">
         <v>143.516998291015</v>
@@ -8599,10 +8598,10 @@
         <v>313</v>
       </c>
       <c r="B152" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C152" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D152">
         <v>-38.623001098632798</v>
@@ -8640,10 +8639,10 @@
         <v>315</v>
       </c>
       <c r="B153" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C153" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="D153">
         <v>-36.206001281738203</v>
@@ -8687,7 +8686,7 @@
         <v>317</v>
       </c>
       <c r="B154" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D154">
         <v>17.7199993133544</v>
@@ -8720,7 +8719,7 @@
         <v>319</v>
       </c>
       <c r="B155" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D155">
         <v>55.332000732421797</v>
@@ -8753,7 +8752,7 @@
         <v>321</v>
       </c>
       <c r="B156" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D156">
         <v>68.579002380371094</v>
@@ -8786,7 +8785,7 @@
         <v>323</v>
       </c>
       <c r="B157" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D157">
         <v>-61.2430000305175</v>
@@ -8816,7 +8815,7 @@
         <v>612</v>
       </c>
       <c r="O157" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="158" spans="1:21" x14ac:dyDescent="0.2">
@@ -8824,10 +8823,10 @@
         <v>325</v>
       </c>
       <c r="B158" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C158" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="D158">
         <v>-81.449996948242102</v>
@@ -8865,10 +8864,10 @@
         <v>327</v>
       </c>
       <c r="B159" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C159" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D159">
         <v>113.480003356933</v>
@@ -8906,10 +8905,10 @@
         <v>329</v>
       </c>
       <c r="B160" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C160" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D160">
         <v>121.78800201416</v>
@@ -8947,7 +8946,7 @@
         <v>331</v>
       </c>
       <c r="B161" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D161">
         <v>141.78300476074199</v>
@@ -8986,7 +8985,7 @@
         <v>333</v>
       </c>
       <c r="B162" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D162">
         <v>-127.036003112792</v>
@@ -9019,10 +9018,10 @@
         <v>335</v>
       </c>
       <c r="B163" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C163" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="D163">
         <v>-91.346000671386705</v>
@@ -9055,10 +9054,10 @@
         <v>611</v>
       </c>
       <c r="S163" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="U163" t="s">
-        <v>665</v>
+        <v>850</v>
       </c>
     </row>
     <row r="164" spans="1:21" x14ac:dyDescent="0.2">
@@ -9066,10 +9065,10 @@
         <v>337</v>
       </c>
       <c r="B164" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C164" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D164">
         <v>17.337999343871999</v>
@@ -9107,7 +9106,7 @@
         <v>339</v>
       </c>
       <c r="B165" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D165">
         <v>136.54800415039</v>
@@ -9137,10 +9136,10 @@
         <v>612</v>
       </c>
       <c r="O165" t="s">
+        <v>666</v>
+      </c>
+      <c r="U165" t="s">
         <v>667</v>
-      </c>
-      <c r="U165" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="166" spans="1:21" x14ac:dyDescent="0.2">
@@ -9148,10 +9147,10 @@
         <v>341</v>
       </c>
       <c r="B166" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C166" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="D166">
         <v>-10.390000343322701</v>
@@ -9189,10 +9188,10 @@
         <v>343</v>
       </c>
       <c r="B167" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C167" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="D167">
         <v>-10.6599998474121</v>
@@ -9222,10 +9221,10 @@
         <v>614</v>
       </c>
       <c r="P167" t="s">
+        <v>724</v>
+      </c>
+      <c r="U167" t="s">
         <v>725</v>
-      </c>
-      <c r="U167" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="168" spans="1:21" x14ac:dyDescent="0.2">
@@ -9233,10 +9232,10 @@
         <v>345</v>
       </c>
       <c r="B168" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C168" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="D168">
         <v>9.3950004577636701</v>
@@ -9274,10 +9273,10 @@
         <v>347</v>
       </c>
       <c r="B169" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C169" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="D169">
         <v>111.44100189208901</v>
@@ -9315,10 +9314,10 @@
         <v>349</v>
       </c>
       <c r="B170" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C170" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="D170">
         <v>111.442001342773</v>
@@ -9356,10 +9355,10 @@
         <v>351</v>
       </c>
       <c r="B171" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C171" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D171">
         <v>116.25299835205</v>
@@ -9397,10 +9396,10 @@
         <v>353</v>
       </c>
       <c r="B172" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C172" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D172">
         <v>151.46000671386699</v>
@@ -9433,7 +9432,7 @@
         <v>611</v>
       </c>
       <c r="U172" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="173" spans="1:21" x14ac:dyDescent="0.2">
@@ -9441,7 +9440,7 @@
         <v>355</v>
       </c>
       <c r="B173" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D173">
         <v>167.89999389648401</v>
@@ -9469,7 +9468,7 @@
       </c>
       <c r="T173"/>
       <c r="U173" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="174" spans="1:21" x14ac:dyDescent="0.2">
@@ -9477,10 +9476,10 @@
         <v>357</v>
       </c>
       <c r="B174" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C174" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D174">
         <v>126.498001098632</v>
@@ -9510,7 +9509,7 @@
         <v>612</v>
       </c>
       <c r="O174" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="175" spans="1:21" x14ac:dyDescent="0.2">
@@ -9518,10 +9517,10 @@
         <v>359</v>
       </c>
       <c r="B175" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C175" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D175">
         <v>125.83200073242099</v>
@@ -9551,10 +9550,10 @@
         <v>612</v>
       </c>
       <c r="O175" t="s">
+        <v>698</v>
+      </c>
+      <c r="U175" t="s">
         <v>699</v>
-      </c>
-      <c r="U175" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="176" spans="1:21" x14ac:dyDescent="0.2">
@@ -9562,7 +9561,7 @@
         <v>361</v>
       </c>
       <c r="B176" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D176">
         <v>-14.227999687194799</v>
@@ -9582,9 +9581,6 @@
       <c r="J176">
         <v>0</v>
       </c>
-      <c r="K176" t="s">
-        <v>830</v>
-      </c>
       <c r="L176">
         <v>59</v>
       </c>
@@ -9595,7 +9591,7 @@
         <v>619</v>
       </c>
       <c r="O176" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="177" spans="1:21" x14ac:dyDescent="0.2">
@@ -9603,7 +9599,7 @@
         <v>363</v>
       </c>
       <c r="B177" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D177">
         <v>-31.1350002288818</v>
@@ -9636,10 +9632,10 @@
         <v>365</v>
       </c>
       <c r="B178" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C178" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="D178">
         <v>128.72000122070301</v>
@@ -9677,7 +9673,7 @@
         <v>367</v>
       </c>
       <c r="B179" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D179">
         <v>51.189998626708899</v>
@@ -9704,7 +9700,7 @@
         <v>1</v>
       </c>
       <c r="U179" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="180" spans="1:21" x14ac:dyDescent="0.2">
@@ -9712,10 +9708,10 @@
         <v>369</v>
       </c>
       <c r="B180" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C180" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="D180">
         <v>72.568000793457003</v>
@@ -9753,7 +9749,7 @@
         <v>371</v>
       </c>
       <c r="B181" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D181">
         <v>36.200000762939403</v>
@@ -9789,7 +9785,7 @@
         <v>373</v>
       </c>
       <c r="B182" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D182">
         <v>51.318000793457003</v>
@@ -9816,7 +9812,7 @@
         <v>1</v>
       </c>
       <c r="U182" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="183" spans="1:21" x14ac:dyDescent="0.2">
@@ -9824,10 +9820,10 @@
         <v>375</v>
       </c>
       <c r="B183" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C183" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D183">
         <v>32.380001068115199</v>
@@ -9865,10 +9861,10 @@
         <v>377</v>
       </c>
       <c r="B184" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C184" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="D184">
         <v>96.460998535156193</v>
@@ -9906,10 +9902,10 @@
         <v>379</v>
       </c>
       <c r="B185" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C185" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="D185">
         <v>9.7690000534057599</v>
@@ -9947,7 +9943,7 @@
         <v>381</v>
       </c>
       <c r="B186" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D186">
         <v>-32.030998229980398</v>
@@ -9975,7 +9971,7 @@
       </c>
       <c r="T186"/>
       <c r="U186" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="187" spans="1:21" x14ac:dyDescent="0.2">
@@ -9983,7 +9979,7 @@
         <v>383</v>
       </c>
       <c r="B187" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D187">
         <v>-10.166999816894499</v>
@@ -10021,10 +10017,10 @@
         <v>385</v>
       </c>
       <c r="B188" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C188" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="D188">
         <v>-2.62100005149841</v>
@@ -10054,7 +10050,7 @@
         <v>619</v>
       </c>
       <c r="P188" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="189" spans="1:21" x14ac:dyDescent="0.2">
@@ -10062,10 +10058,10 @@
         <v>387</v>
       </c>
       <c r="B189" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C189" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="D189">
         <v>12.6300001144409</v>
@@ -10095,7 +10091,7 @@
         <v>624</v>
       </c>
       <c r="O189" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="190" spans="1:21" x14ac:dyDescent="0.2">
@@ -10103,10 +10099,10 @@
         <v>389</v>
       </c>
       <c r="B190" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C190" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="D190">
         <v>146.28500366210901</v>
@@ -10144,7 +10140,7 @@
         <v>391</v>
       </c>
       <c r="B191" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D191">
         <v>177.99499511718699</v>
@@ -10177,10 +10173,10 @@
         <v>393</v>
       </c>
       <c r="B192" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C192" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="D192">
         <v>146.13999938964801</v>
@@ -10218,10 +10214,10 @@
         <v>395</v>
       </c>
       <c r="B193" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C193" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="D193">
         <v>109.869003295898</v>
@@ -10259,7 +10255,7 @@
         <v>397</v>
       </c>
       <c r="B194" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D194">
         <v>133.44000244140599</v>
@@ -10287,7 +10283,7 @@
       </c>
       <c r="T194"/>
       <c r="U194" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="195" spans="1:21" x14ac:dyDescent="0.2">
@@ -10295,7 +10291,7 @@
         <v>399</v>
       </c>
       <c r="B195" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D195">
         <v>125.81999969482401</v>
@@ -10328,7 +10324,7 @@
         <v>620</v>
       </c>
       <c r="S195" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="196" spans="1:21" x14ac:dyDescent="0.2">
@@ -10336,7 +10332,7 @@
         <v>401</v>
       </c>
       <c r="B196" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D196">
         <v>-7.5279998779296804</v>
@@ -10366,10 +10362,10 @@
         <v>612</v>
       </c>
       <c r="O196" t="s">
+        <v>692</v>
+      </c>
+      <c r="U196" t="s">
         <v>693</v>
-      </c>
-      <c r="U196" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="197" spans="1:21" x14ac:dyDescent="0.2">
@@ -10377,7 +10373,7 @@
         <v>403</v>
       </c>
       <c r="B197" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D197">
         <v>4.0279998779296804</v>
@@ -10407,10 +10403,10 @@
         <v>614</v>
       </c>
       <c r="P197" t="s">
+        <v>684</v>
+      </c>
+      <c r="U197" t="s">
         <v>685</v>
-      </c>
-      <c r="U197" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.2">
@@ -10418,7 +10414,7 @@
         <v>405</v>
       </c>
       <c r="B198" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D198">
         <v>-86.459999084472599</v>
@@ -10445,7 +10441,7 @@
         <v>1</v>
       </c>
       <c r="U198" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="199" spans="1:21" x14ac:dyDescent="0.2">
@@ -10453,7 +10449,7 @@
         <v>407</v>
       </c>
       <c r="B199" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D199">
         <v>-83.608001708984304</v>
@@ -10486,10 +10482,10 @@
         <v>409</v>
       </c>
       <c r="B200" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C200" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="D200">
         <v>-155.96000671386699</v>
@@ -10527,10 +10523,10 @@
         <v>411</v>
       </c>
       <c r="B201" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C201" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="D201">
         <v>-156.66000366210901</v>
@@ -10560,7 +10556,7 @@
         <v>612</v>
       </c>
       <c r="P201" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="202" spans="1:21" x14ac:dyDescent="0.2">
@@ -10568,7 +10564,7 @@
         <v>413</v>
       </c>
       <c r="B202" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D202">
         <v>-157.259994506835</v>
@@ -10603,10 +10599,10 @@
         <v>415</v>
       </c>
       <c r="B203" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C203" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="D203">
         <v>-159.28999328613199</v>
@@ -10636,7 +10632,7 @@
         <v>612</v>
       </c>
       <c r="P203" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="204" spans="1:21" x14ac:dyDescent="0.2">
@@ -10644,10 +10640,10 @@
         <v>417</v>
       </c>
       <c r="B204" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C204" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="D204">
         <v>-159.19999694824199</v>
@@ -10677,7 +10673,7 @@
         <v>612</v>
       </c>
       <c r="P204" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="205" spans="1:21" x14ac:dyDescent="0.2">
@@ -10685,10 +10681,10 @@
         <v>419</v>
       </c>
       <c r="B205" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C205" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="D205">
         <v>-160.05000305175699</v>
@@ -10721,10 +10717,10 @@
         <v>611</v>
       </c>
       <c r="T205" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="U205" t="s">
         <v>742</v>
-      </c>
-      <c r="U205" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="206" spans="1:21" x14ac:dyDescent="0.2">
@@ -10732,7 +10728,7 @@
         <v>421</v>
       </c>
       <c r="B206" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D206">
         <v>-160.42999267578099</v>
@@ -10767,10 +10763,10 @@
         <v>423</v>
       </c>
       <c r="B207" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C207" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="D207">
         <v>-161.03999328613199</v>
@@ -10800,7 +10796,7 @@
         <v>612</v>
       </c>
       <c r="P207" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="208" spans="1:21" x14ac:dyDescent="0.2">
@@ -10808,10 +10804,10 @@
         <v>425</v>
       </c>
       <c r="B208" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C208" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="D208">
         <v>-161.63000488281199</v>
@@ -10849,10 +10845,10 @@
         <v>427</v>
       </c>
       <c r="B209" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C209" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D209">
         <v>152.53300476074199</v>
@@ -10890,7 +10886,7 @@
         <v>429</v>
       </c>
       <c r="B210" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D210">
         <v>153.016998291015</v>
@@ -10923,7 +10919,7 @@
         <v>431</v>
       </c>
       <c r="B211" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D211">
         <v>31.649999618530199</v>
@@ -10953,7 +10949,7 @@
         <v>612</v>
       </c>
       <c r="U211" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="212" spans="1:21" x14ac:dyDescent="0.2">
@@ -10961,7 +10957,7 @@
         <v>433</v>
       </c>
       <c r="B212" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D212">
         <v>158.940994262695</v>
@@ -10994,10 +10990,10 @@
         <v>435</v>
       </c>
       <c r="B213" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C213" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D213">
         <v>161.003005981445</v>
@@ -11027,10 +11023,10 @@
         <v>608</v>
       </c>
       <c r="O213" t="s">
+        <v>680</v>
+      </c>
+      <c r="U213" t="s">
         <v>681</v>
-      </c>
-      <c r="U213" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="214" spans="1:21" x14ac:dyDescent="0.2">
@@ -11038,7 +11034,7 @@
         <v>437</v>
       </c>
       <c r="B214" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D214">
         <v>161.77299499511699</v>
@@ -11071,10 +11067,10 @@
         <v>439</v>
       </c>
       <c r="B215" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C215" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D215">
         <v>-78.027999877929602</v>
@@ -11112,7 +11108,7 @@
         <v>441</v>
       </c>
       <c r="B216" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D216">
         <v>-18.580999374389599</v>
@@ -11142,7 +11138,7 @@
         <v>619</v>
       </c>
       <c r="U216" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="217" spans="1:21" x14ac:dyDescent="0.2">
@@ -11150,7 +11146,7 @@
         <v>443</v>
       </c>
       <c r="B217" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D217">
         <v>121.294998168945</v>
@@ -11177,7 +11173,7 @@
         <v>1</v>
       </c>
       <c r="U217" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="218" spans="1:21" x14ac:dyDescent="0.2">
@@ -11185,7 +11181,7 @@
         <v>445</v>
       </c>
       <c r="B218" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D218">
         <v>-177.99699401855401</v>
@@ -11221,7 +11217,7 @@
         <v>447</v>
       </c>
       <c r="B219" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D219">
         <v>177.24200439453099</v>
@@ -11256,7 +11252,7 @@
         <v>449</v>
       </c>
       <c r="B220" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D220">
         <v>-102.453002929687</v>
@@ -11286,10 +11282,10 @@
         <v>612</v>
       </c>
       <c r="O220" t="s">
+        <v>729</v>
+      </c>
+      <c r="U220" t="s">
         <v>730</v>
-      </c>
-      <c r="U220" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="221" spans="1:21" x14ac:dyDescent="0.2">
@@ -11297,10 +11293,10 @@
         <v>451</v>
       </c>
       <c r="B221" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C221" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D221">
         <v>-9.5030002593994105</v>
@@ -11338,10 +11334,10 @@
         <v>453</v>
       </c>
       <c r="B222" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C222" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D222">
         <v>-14.4899997711181</v>
@@ -11379,10 +11375,10 @@
         <v>455</v>
       </c>
       <c r="B223" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C223" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D223">
         <v>-14.227999687194799</v>
@@ -11420,7 +11416,7 @@
         <v>457</v>
       </c>
       <c r="B224" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D224">
         <v>-15.333000183105399</v>
@@ -11458,7 +11454,7 @@
         <v>459</v>
       </c>
       <c r="B225" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D225">
         <v>28.541700363159102</v>
@@ -11496,10 +11492,10 @@
         <v>461</v>
       </c>
       <c r="B226" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C226" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D226">
         <v>-85.817001342773395</v>
@@ -11537,7 +11533,7 @@
         <v>463</v>
       </c>
       <c r="B227" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D227">
         <v>9.8000001907348597</v>
@@ -11575,7 +11571,7 @@
         <v>465</v>
       </c>
       <c r="B228" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D228">
         <v>96.067001342773395</v>
@@ -11608,10 +11604,10 @@
         <v>467</v>
       </c>
       <c r="B229" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C229" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D229">
         <v>-87.75</v>
@@ -11649,10 +11645,10 @@
         <v>469</v>
       </c>
       <c r="B230" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C230" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D230">
         <v>-46.509998321533203</v>
@@ -11690,7 +11686,7 @@
         <v>471</v>
       </c>
       <c r="B231" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D231">
         <v>-43.330001831054602</v>
@@ -11723,7 +11719,7 @@
         <v>473</v>
       </c>
       <c r="B232" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D232">
         <v>158.80000305175699</v>
@@ -11761,7 +11757,7 @@
         <v>475</v>
       </c>
       <c r="B233" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D233">
         <v>-86.849998474121094</v>
@@ -11799,10 +11795,10 @@
         <v>477</v>
       </c>
       <c r="B234" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C234" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D234">
         <v>168.31199645996</v>
@@ -11832,10 +11828,10 @@
         <v>619</v>
       </c>
       <c r="O234" t="s">
+        <v>682</v>
+      </c>
+      <c r="U234" t="s">
         <v>683</v>
-      </c>
-      <c r="U234" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="235" spans="1:21" x14ac:dyDescent="0.2">
@@ -11843,7 +11839,7 @@
         <v>479</v>
       </c>
       <c r="B235" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D235">
         <v>153.85200500488199</v>
@@ -11876,7 +11872,7 @@
         <v>481</v>
       </c>
       <c r="B236" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D236">
         <v>152</v>
@@ -11909,7 +11905,7 @@
         <v>483</v>
       </c>
       <c r="B237" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D237">
         <v>151.92300415039</v>
@@ -11942,10 +11938,10 @@
         <v>485</v>
       </c>
       <c r="B238" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C238" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="D238">
         <v>146.28300476074199</v>
@@ -11983,7 +11979,7 @@
         <v>487</v>
       </c>
       <c r="B239" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D239">
         <v>-42.279998779296797</v>
@@ -12016,7 +12012,7 @@
         <v>489</v>
       </c>
       <c r="B240" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D240">
         <v>111.494003295898</v>
@@ -12044,7 +12040,7 @@
       </c>
       <c r="T240"/>
       <c r="U240" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="241" spans="1:21" x14ac:dyDescent="0.2">
@@ -12052,10 +12048,10 @@
         <v>491</v>
       </c>
       <c r="B241" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C241" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D241">
         <v>-10.149999618530201</v>
@@ -12093,7 +12089,7 @@
         <v>493</v>
       </c>
       <c r="B242" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D242">
         <v>90.25</v>
@@ -12126,7 +12122,7 @@
         <v>495</v>
       </c>
       <c r="B243" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D243">
         <v>90.300003051757798</v>
@@ -12159,7 +12155,7 @@
         <v>497</v>
       </c>
       <c r="B244" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D244">
         <v>88.699996948242102</v>
@@ -12192,7 +12188,7 @@
         <v>499</v>
       </c>
       <c r="B245" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D245">
         <v>78</v>
@@ -12225,10 +12221,10 @@
         <v>501</v>
       </c>
       <c r="B246" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C246" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D246">
         <v>82.001998901367102</v>
@@ -12266,7 +12262,7 @@
         <v>503</v>
       </c>
       <c r="B247" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D247">
         <v>74.999000549316406</v>
@@ -12299,7 +12295,7 @@
         <v>505</v>
       </c>
       <c r="B248" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D248">
         <v>70.870002746582003</v>
@@ -12332,7 +12328,7 @@
         <v>507</v>
       </c>
       <c r="B249" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D249">
         <v>-74.697998046875</v>
@@ -12365,7 +12361,7 @@
         <v>509</v>
       </c>
       <c r="B250" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D250">
         <v>-72.209999084472599</v>
@@ -12398,7 +12394,7 @@
         <v>511</v>
       </c>
       <c r="B251" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D251">
         <v>-116.87899780273401</v>
@@ -12431,10 +12427,10 @@
         <v>513</v>
       </c>
       <c r="B252" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C252" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="D252">
         <v>176.60200500488199</v>
@@ -12472,7 +12468,7 @@
         <v>515</v>
       </c>
       <c r="B253" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D253">
         <v>-165.05299377441401</v>
@@ -12510,7 +12506,7 @@
         <v>517</v>
       </c>
       <c r="B254" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D254">
         <v>-162.13800048828099</v>
@@ -12543,10 +12539,10 @@
         <v>519</v>
       </c>
       <c r="B255" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C255" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D255">
         <v>60.251998901367102</v>
@@ -12579,10 +12575,10 @@
         <v>521</v>
       </c>
       <c r="B256" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C256" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D256">
         <v>63.122001647949197</v>
@@ -12610,7 +12606,7 @@
       </c>
       <c r="T256"/>
       <c r="U256" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="257" spans="1:21" x14ac:dyDescent="0.2">
@@ -12618,10 +12614,10 @@
         <v>523</v>
       </c>
       <c r="B257" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C257" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D257">
         <v>57.347000122070298</v>
@@ -12659,10 +12655,10 @@
         <v>525</v>
       </c>
       <c r="B258" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C258" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="D258">
         <v>-9.5030002593994105</v>
@@ -12692,10 +12688,10 @@
         <v>619</v>
       </c>
       <c r="O258" t="s">
+        <v>700</v>
+      </c>
+      <c r="U258" t="s">
         <v>701</v>
-      </c>
-      <c r="U258" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="259" spans="1:21" x14ac:dyDescent="0.2">
@@ -12703,10 +12699,10 @@
         <v>527</v>
       </c>
       <c r="B259" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C259" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D259">
         <v>170.16700744628901</v>
@@ -12744,10 +12740,10 @@
         <v>529</v>
       </c>
       <c r="B260" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C260" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D260">
         <v>-10.182999610900801</v>
@@ -12785,7 +12781,7 @@
         <v>531</v>
       </c>
       <c r="B261" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D261">
         <v>166.06100463867099</v>
@@ -12818,7 +12814,7 @@
         <v>533</v>
       </c>
       <c r="B262" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D262">
         <v>164.60899353027301</v>
@@ -12851,7 +12847,7 @@
         <v>535</v>
       </c>
       <c r="B263" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D263">
         <v>166.649002075195</v>
@@ -12884,7 +12880,7 @@
         <v>537</v>
       </c>
       <c r="B264" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D264">
         <v>166.01300048828099</v>
@@ -12917,7 +12913,7 @@
         <v>539</v>
       </c>
       <c r="B265" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D265">
         <v>165.65899658203099</v>
@@ -12950,7 +12946,7 @@
         <v>541</v>
       </c>
       <c r="B266" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D266">
         <v>165.16600036621</v>
@@ -12983,7 +12979,7 @@
         <v>543</v>
       </c>
       <c r="B267" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D267">
         <v>122.62200164794901</v>
@@ -13016,7 +13012,7 @@
         <v>545</v>
       </c>
       <c r="B268" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D268">
         <v>-88.449996948242102</v>
@@ -13046,7 +13042,7 @@
         <v>621</v>
       </c>
       <c r="P268" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="269" spans="1:21" x14ac:dyDescent="0.2">
@@ -13054,10 +13050,10 @@
         <v>547</v>
       </c>
       <c r="B269" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C269" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D269">
         <v>130.99800109863199</v>
@@ -13095,10 +13091,10 @@
         <v>549</v>
       </c>
       <c r="B270" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C270" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D270">
         <v>131</v>
@@ -13136,10 +13132,10 @@
         <v>551</v>
       </c>
       <c r="B271" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C271" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D271">
         <v>-82.067001342773395</v>
@@ -13177,10 +13173,10 @@
         <v>553</v>
       </c>
       <c r="B272" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C272" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D272">
         <v>-84.650001525878906</v>
@@ -13218,7 +13214,7 @@
         <v>555</v>
       </c>
       <c r="B273" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D273">
         <v>-33.029998779296797</v>
@@ -13256,10 +13252,10 @@
         <v>557</v>
       </c>
       <c r="B274" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C274" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D274">
         <v>-106.766998291015</v>
@@ -13297,7 +13293,7 @@
         <v>559</v>
       </c>
       <c r="B275" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D275">
         <v>-44.680000305175703</v>
@@ -13324,13 +13320,13 @@
         <v>1</v>
       </c>
       <c r="N275" t="s">
+        <v>732</v>
+      </c>
+      <c r="O275" t="s">
         <v>733</v>
       </c>
-      <c r="O275" t="s">
+      <c r="U275" t="s">
         <v>734</v>
-      </c>
-      <c r="U275" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="276" spans="1:21" x14ac:dyDescent="0.2">
@@ -13338,7 +13334,7 @@
         <v>561</v>
       </c>
       <c r="B276" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D276">
         <v>-72.379997253417898</v>
@@ -13371,10 +13367,10 @@
         <v>563</v>
       </c>
       <c r="B277" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C277" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="D277">
         <v>-78.680000305175696</v>
@@ -13407,7 +13403,7 @@
         <v>611</v>
       </c>
       <c r="U277" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="278" spans="1:21" x14ac:dyDescent="0.2">
@@ -13415,10 +13411,10 @@
         <v>565</v>
       </c>
       <c r="B278" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C278" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D278">
         <v>150.46000671386699</v>
@@ -13456,7 +13452,7 @@
         <v>567</v>
       </c>
       <c r="B279" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D279">
         <v>-66.629997253417898</v>
@@ -13489,10 +13485,10 @@
         <v>569</v>
       </c>
       <c r="B280" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C280" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D280">
         <v>140.100006103515</v>
@@ -13530,7 +13526,7 @@
         <v>571</v>
       </c>
       <c r="B281" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D281">
         <v>156.69999694824199</v>
@@ -13568,7 +13564,7 @@
         <v>573</v>
       </c>
       <c r="B282" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D282">
         <v>155.69999694824199</v>
@@ -13606,7 +13602,7 @@
         <v>575</v>
       </c>
       <c r="B283" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D283">
         <v>176.19999694824199</v>
@@ -13644,7 +13640,7 @@
         <v>577</v>
       </c>
       <c r="B284" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D284">
         <v>168.69999694824199</v>
@@ -13682,7 +13678,7 @@
         <v>579</v>
       </c>
       <c r="B285" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D285">
         <v>167.80000305175699</v>
@@ -13720,7 +13716,7 @@
         <v>581</v>
       </c>
       <c r="B286" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D286">
         <v>166.80000305175699</v>
@@ -13758,7 +13754,7 @@
         <v>583</v>
       </c>
       <c r="B287" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D287">
         <v>161.39999389648401</v>
@@ -13796,10 +13792,10 @@
         <v>585</v>
       </c>
       <c r="B288" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C288" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D288">
         <v>159</v>
@@ -13829,7 +13825,7 @@
         <v>613</v>
       </c>
       <c r="P288" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="289" spans="1:21" x14ac:dyDescent="0.2">
@@ -13837,7 +13833,7 @@
         <v>587</v>
       </c>
       <c r="B289" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D289">
         <v>160.5</v>
@@ -13875,7 +13871,7 @@
         <v>589</v>
       </c>
       <c r="B290" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D290">
         <v>160.5</v>
@@ -13913,7 +13909,7 @@
         <v>591</v>
       </c>
       <c r="B291" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D291">
         <v>162</v>
@@ -13951,10 +13947,10 @@
         <v>593</v>
       </c>
       <c r="B292" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C292" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D292">
         <v>142.69999694824199</v>
@@ -13992,7 +13988,7 @@
         <v>595</v>
       </c>
       <c r="B293" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D293">
         <v>176.100006103515</v>
@@ -14030,10 +14026,10 @@
         <v>597</v>
       </c>
       <c r="B294" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C294" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D294">
         <v>-102.014999389648</v>
@@ -14071,7 +14067,7 @@
         <v>599</v>
       </c>
       <c r="B295" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D295">
         <v>-125.75</v>
@@ -14101,7 +14097,7 @@
         <v>619</v>
       </c>
       <c r="U295" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="296" spans="1:21" x14ac:dyDescent="0.2">
@@ -14109,7 +14105,7 @@
         <v>601</v>
       </c>
       <c r="B296" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D296">
         <v>-127.678001403808</v>
@@ -14137,7 +14133,7 @@
       </c>
       <c r="T296"/>
       <c r="U296" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="297" spans="1:21" x14ac:dyDescent="0.2">
@@ -14145,7 +14141,7 @@
         <v>603</v>
       </c>
       <c r="B297" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D297">
         <v>-127.678001403808</v>
@@ -14173,7 +14169,7 @@
       </c>
       <c r="T297"/>
       <c r="U297" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="298" spans="1:21" x14ac:dyDescent="0.2">
@@ -14181,10 +14177,10 @@
         <v>605</v>
       </c>
       <c r="B298" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C298" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D298">
         <v>51.0130004882812</v>

</xml_diff>